<commit_message>
added continual spawning and ability to choose heritage.
</commit_message>
<xml_diff>
--- a/app/resources/Game_Data.xlsx
+++ b/app/resources/Game_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
@@ -10114,8 +10114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R403"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10449,7 +10449,7 @@
         <v>29</v>
       </c>
       <c r="E8">
-        <f t="shared" si="3"/>
+        <f>E7+5</f>
         <v>25</v>
       </c>
       <c r="F8">
@@ -29809,7 +29809,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -47933,8 +47933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C502"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -50477,7 +50477,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -50522,7 +50522,7 @@
   <dimension ref="A1:T127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>